<commit_message>
case : change controller
</commit_message>
<xml_diff>
--- a/uploads/formatexcel_user.xlsx
+++ b/uploads/formatexcel_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\first\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8CED04-97EB-4060-B129-437775E57E5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1021C67-C4FB-45BE-8E99-D6ABD4402EAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ID_Employee</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>x007</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>